<commit_message>
modified:   app.py 	modified:   bayern-bvb-fichajes-filtro@3.xlsx
</commit_message>
<xml_diff>
--- a/bayern-bvb-fichajes-filtro@3.xlsx
+++ b/bayern-bvb-fichajes-filtro@3.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FCBBVB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF2F3B17-9994-4217-B784-913E20332BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BD625C9-4396-476A-86CE-F760D63D96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A14204A7-E8F8-4E7D-9E9B-DC80553F3DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="bayern bvb fichajes filtro@2 xl" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'bayern bvb fichajes filtro@2 xl'!$A$1:$H$495</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="603">
   <si>
     <t>Jugador</t>
   </si>
@@ -1754,27 +1757,108 @@
   </si>
   <si>
     <t>Atlético-MG</t>
+  </si>
+  <si>
+    <t>Michael Olise</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Hiroki Ito</t>
+  </si>
+  <si>
+    <t>Bryan Zaragoza</t>
+  </si>
+  <si>
+    <t>Nestory Irankunda</t>
+  </si>
+  <si>
+    <t>Adelaide United</t>
+  </si>
+  <si>
+    <t>Armindo Sieb</t>
+  </si>
+  <si>
+    <t>Maurice Krattenmacher</t>
+  </si>
+  <si>
+    <t>Gibson Nana Adu</t>
+  </si>
+  <si>
+    <t>Lovro Zvonarek</t>
+  </si>
+  <si>
+    <t>Adam Aznou</t>
+  </si>
+  <si>
+    <t>Noel Aséko Nkili</t>
+  </si>
+  <si>
+    <t>B. Leverkusen</t>
+  </si>
+  <si>
+    <t>SV Elversberg</t>
+  </si>
+  <si>
+    <t>Frosinone</t>
+  </si>
+  <si>
+    <t>Dinamo Zagreb</t>
+  </si>
+  <si>
+    <t>SuperSport HNL</t>
+  </si>
+  <si>
+    <t>Austria Wien</t>
+  </si>
+  <si>
+    <t>Joao Palhinha</t>
+  </si>
+  <si>
+    <t>Waldemar Anton</t>
+  </si>
+  <si>
+    <t>Serhou Guirassy</t>
+  </si>
+  <si>
+    <t>Nottm Forest</t>
+  </si>
+  <si>
+    <t>Holstein Kiel</t>
+  </si>
+  <si>
+    <t>Royal Antwerpen</t>
+  </si>
+  <si>
+    <t>Belgien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1782,18 +1866,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B484E89F-EDB7-47CD-B86C-6EB668A85E54}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2122,9 +2251,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A416F442-7BFC-4C4B-B75D-F8A8152172F9}">
-  <dimension ref="A1:H495"/>
+  <dimension ref="A1:H519"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A495" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H515" sqref="H515:H519"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15001,9 +15132,634 @@
         <v>2001</v>
       </c>
     </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A496" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B496" s="2">
+        <v>22</v>
+      </c>
+      <c r="C496" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D496" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E496" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F496" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G496" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H496">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A497" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="B497" s="5">
+        <v>29</v>
+      </c>
+      <c r="C497" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="D497" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E497" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F497" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G497" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H497">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B498" s="2">
+        <v>25</v>
+      </c>
+      <c r="C498" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D498" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E498" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F498" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G498" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H498">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A499" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="B499" s="5">
+        <v>22</v>
+      </c>
+      <c r="C499" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="D499" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E499" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F499" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G499" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H499">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A500" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B500" s="2">
+        <v>18</v>
+      </c>
+      <c r="C500" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D500" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E500" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F500" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G500" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H500">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A501" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B501" s="5">
+        <v>21</v>
+      </c>
+      <c r="C501" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D501" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E501" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F501" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G501" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H501">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A502" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B502" s="2">
+        <v>30</v>
+      </c>
+      <c r="C502" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D502" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E502" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F502" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G502" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H502">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A503" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B503" s="5">
+        <v>18</v>
+      </c>
+      <c r="C503" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D503" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E503" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F503" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G503" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H503">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A504" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B504" s="2">
+        <v>16</v>
+      </c>
+      <c r="C504" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D504" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E504" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F504" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G504" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H504">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A505" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="B505" s="5">
+        <v>19</v>
+      </c>
+      <c r="C505" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D505" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E505" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F505" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G505" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H505">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B506" s="2">
+        <v>18</v>
+      </c>
+      <c r="C506" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D506" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E506" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F506" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G506" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H506">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A507" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B507" s="5">
+        <v>18</v>
+      </c>
+      <c r="C507" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D507" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E507" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F507" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G507" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H507">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B508" s="2">
+        <v>24</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D508" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E508" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F508" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G508" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H508">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A509" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B509" s="5">
+        <v>22</v>
+      </c>
+      <c r="C509" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D509" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E509" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F509" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G509" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H509">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B510" s="2">
+        <v>18</v>
+      </c>
+      <c r="C510" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D510" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E510" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F510" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G510" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H510">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A511" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B511" s="5">
+        <v>18</v>
+      </c>
+      <c r="C511" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="D511" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E511" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F511" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G511" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H511">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B512" s="2">
+        <v>20</v>
+      </c>
+      <c r="C512" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="D512" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E512" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="F512" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G512" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H512">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A513" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B513" s="5">
+        <v>21</v>
+      </c>
+      <c r="C513" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D513" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E513" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F513" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G513" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H513">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B514" s="2">
+        <v>21</v>
+      </c>
+      <c r="C514" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D514" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E514" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F514" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G514" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H514">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B515" s="2">
+        <v>27</v>
+      </c>
+      <c r="C515" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D515" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E515" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F515" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G515" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H515">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A516" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B516" s="5">
+        <v>28</v>
+      </c>
+      <c r="C516" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D516" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E516" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F516" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G516" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H516">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B517" s="2">
+        <v>21</v>
+      </c>
+      <c r="C517" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="D517" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E517" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F517" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G517" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H517">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A518" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B518" s="5">
+        <v>19</v>
+      </c>
+      <c r="C518" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D518" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F518" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G518" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H518">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B519" s="2">
+        <v>20</v>
+      </c>
+      <c r="C519" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="D519" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E519" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="F519" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G519" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H519">
+        <v>2024</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H495" xr:uid="{A416F442-7BFC-4C4B-B75D-F8A8152172F9}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   .vscode/settings.json     modified:   bayern-bvb-fichajes-filtro@3.xlsx
</commit_message>
<xml_diff>
--- a/bayern-bvb-fichajes-filtro@3.xlsx
+++ b/bayern-bvb-fichajes-filtro@3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FCBBVB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BD625C9-4396-476A-86CE-F760D63D96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB88747-F547-4D8D-A770-89AF4877C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A14204A7-E8F8-4E7D-9E9B-DC80553F3DB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A14204A7-E8F8-4E7D-9E9B-DC80553F3DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="bayern bvb fichajes filtro@2 xl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="605">
   <si>
     <t>Jugador</t>
   </si>
@@ -1832,6 +1832,12 @@
   </si>
   <si>
     <t>Belgien</t>
+  </si>
+  <si>
+    <t>Pascal Groß</t>
+  </si>
+  <si>
+    <t>Brighton &amp; Holve Albion</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1903,11 +1909,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1915,6 +1939,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2251,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A416F442-7BFC-4C4B-B75D-F8A8152172F9}">
-  <dimension ref="A1:H519"/>
+  <dimension ref="A1:H520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A495" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H515" sqref="H515:H519"/>
+    <sheetView tabSelected="1" topLeftCell="A508" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H520" sqref="H520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15756,6 +15783,32 @@
         <v>2024</v>
       </c>
     </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A520" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="B520" s="8">
+        <v>33</v>
+      </c>
+      <c r="C520" s="8" t="s">
+        <v>604</v>
+      </c>
+      <c r="D520" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E520" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F520" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G520" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H520">
+        <v>2024</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H495" xr:uid="{A416F442-7BFC-4C4B-B75D-F8A8152172F9}"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modified:   appv4.py 	modified:   bayern-bvb-fichajes-filtro@3.xlsx
</commit_message>
<xml_diff>
--- a/bayern-bvb-fichajes-filtro@3.xlsx
+++ b/bayern-bvb-fichajes-filtro@3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FCBBVB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB88747-F547-4D8D-A770-89AF4877C8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5840800-0142-409A-A48A-304D173931E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A14204A7-E8F8-4E7D-9E9B-DC80553F3DB7}"/>
   </bookViews>
@@ -1931,7 +1931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1939,9 +1939,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2280,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A416F442-7BFC-4C4B-B75D-F8A8152172F9}">
   <dimension ref="A1:H520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A508" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H520" sqref="H520"/>
     </sheetView>
   </sheetViews>
@@ -15787,22 +15786,22 @@
       <c r="A520" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="B520" s="8">
+      <c r="B520">
         <v>33</v>
       </c>
-      <c r="C520" s="8" t="s">
+      <c r="C520" t="s">
         <v>604</v>
       </c>
-      <c r="D520" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E520" s="8" t="s">
+      <c r="D520" t="s">
+        <v>62</v>
+      </c>
+      <c r="E520" t="s">
         <v>153</v>
       </c>
-      <c r="F520" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G520" s="9" t="s">
+      <c r="F520" t="s">
+        <v>12</v>
+      </c>
+      <c r="G520" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H520">

</xml_diff>